<commit_message>
General update to Python3 and ArcPro
</commit_message>
<xml_diff>
--- a/LifespanDesign/.templates/threshold_values.xlsx
+++ b/LifespanDesign/.templates/threshold_values.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="83">
   <si>
     <t>Flow depth</t>
   </si>
@@ -194,9 +194,6 @@
     <t>bedrock, hillside</t>
   </si>
   <si>
-    <t>tributary channel, tributary delta</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
   </si>
   <si>
     <t>bank, floodplain, high floodplain, island-floodplain, island high floodplain, in-channel bar, lateral bar, levee, spur dike, terrace</t>
-  </si>
-  <si>
-    <t>riffle, riffle transition, pool, floodplain, island floodplain, in-channel bar, lateral bar, medial bar, run</t>
   </si>
   <si>
     <t>agriplain, backswamp, mining pit, pond, slackwater</t>
@@ -526,7 +520,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="163">
+  <borders count="162">
     <border>
       <left/>
       <right/>
@@ -2539,17 +2533,6 @@
       <right style="thin">
         <color theme="3" tint="0.39976195562608724"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -2834,7 +2817,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="300">
+  <cellXfs count="299">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3525,16 +3508,13 @@
     <xf numFmtId="2" fontId="5" fillId="3" borderId="141" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="11" borderId="142" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="143" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="142" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="11" borderId="143" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="14" fillId="11" borderId="144" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="11" borderId="145" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3543,53 +3523,53 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="146" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="145" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="145" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="146" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="147" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="147" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="148" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="149" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="130" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="153" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="152" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="132" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="153" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="154" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="155" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="154" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="155" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="156" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="153" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="154" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="155" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="156" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="156" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="155" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="157" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="158" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="159" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="160" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="158" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="161" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="159" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="157" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="160" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3619,8 +3599,17 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="123" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="162" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="161" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="157" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="158" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="160" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3640,19 +3629,22 @@
     <xf numFmtId="0" fontId="14" fillId="11" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="157" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="156" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="131" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="149" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="150" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="151" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="152" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="149" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="150" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3661,7 +3653,7 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="151" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="152" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="149" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="150" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3670,7 +3662,7 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="151" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="152" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="149" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="150" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3678,18 +3670,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="151" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="152" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="158" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="159" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="161" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3988,7 +3968,7 @@
   <dimension ref="B1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4015,168 +3995,168 @@
   <sheetData>
     <row r="1" spans="2:19" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E2" s="285" t="s">
+      <c r="E2" s="287" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="288"/>
+      <c r="G2" s="288"/>
+      <c r="H2" s="288"/>
+      <c r="I2" s="289"/>
+      <c r="J2" s="290" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="291"/>
+      <c r="L2" s="291"/>
+      <c r="M2" s="292"/>
+      <c r="N2" s="293" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="287"/>
-      <c r="J2" s="288" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="289"/>
-      <c r="L2" s="289"/>
-      <c r="M2" s="290"/>
-      <c r="N2" s="291" t="s">
-        <v>77</v>
-      </c>
-      <c r="O2" s="292"/>
-      <c r="P2" s="293"/>
-      <c r="Q2" s="294" t="s">
-        <v>76</v>
-      </c>
-      <c r="R2" s="295"/>
-      <c r="S2" s="296"/>
+      <c r="O2" s="294"/>
+      <c r="P2" s="295"/>
+      <c r="Q2" s="296" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="297"/>
+      <c r="S2" s="298"/>
     </row>
     <row r="3" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="251"/>
-      <c r="C3" s="252" t="s">
+      <c r="B3" s="250"/>
+      <c r="C3" s="251" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="253" t="s">
+      <c r="D3" s="252" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="254"/>
-      <c r="F3" s="255"/>
-      <c r="G3" s="255"/>
-      <c r="H3" s="256"/>
-      <c r="I3" s="257"/>
-      <c r="J3" s="258"/>
-      <c r="K3" s="259"/>
-      <c r="L3" s="259"/>
-      <c r="M3" s="260"/>
-      <c r="N3" s="254"/>
-      <c r="O3" s="256"/>
-      <c r="P3" s="261"/>
-      <c r="Q3" s="283" t="s">
+      <c r="E3" s="253"/>
+      <c r="F3" s="254"/>
+      <c r="G3" s="254"/>
+      <c r="H3" s="255"/>
+      <c r="I3" s="256"/>
+      <c r="J3" s="257"/>
+      <c r="K3" s="258"/>
+      <c r="L3" s="258"/>
+      <c r="M3" s="259"/>
+      <c r="N3" s="253"/>
+      <c r="O3" s="255"/>
+      <c r="P3" s="260"/>
+      <c r="Q3" s="285" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="284"/>
-      <c r="S3" s="276" t="s">
-        <v>79</v>
+      <c r="R3" s="286"/>
+      <c r="S3" s="275" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="267" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="268" t="s">
+      <c r="B4" s="266" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="267" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="269" t="s">
+      <c r="D4" s="268" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="270" t="s">
+      <c r="E4" s="269" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="270" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="270" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="271" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="272" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="269" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="270" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="270" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="273" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="269" t="s">
+        <v>72</v>
+      </c>
+      <c r="O4" s="271" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="272" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q4" s="274" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="271" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="271" t="s">
+      <c r="R4" s="267" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="272" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="273" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="270" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="271" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" s="271" t="s">
-        <v>54</v>
-      </c>
-      <c r="M4" s="274" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" s="270" t="s">
-        <v>74</v>
-      </c>
-      <c r="O4" s="272" t="s">
+      <c r="S4" s="272" t="s">
         <v>82</v>
-      </c>
-      <c r="P4" s="273" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q4" s="275" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="268" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" s="273" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="262" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="263" t="s">
+      <c r="B5" s="261" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="262" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="264" t="s">
+      <c r="D5" s="263" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="297" t="s">
+      <c r="E5" s="276" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="277" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="277" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="298" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="298" t="s">
+      <c r="H5" s="277" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="278" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="264" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="262" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="262" t="s">
+        <v>62</v>
+      </c>
+      <c r="M5" s="265" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="276" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" s="277" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="278" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q5" s="276" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" s="277" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="298" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="299" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" s="265" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" s="263" t="s">
-        <v>63</v>
-      </c>
-      <c r="L5" s="263" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="266" t="s">
-        <v>65</v>
-      </c>
-      <c r="N5" s="297" t="s">
-        <v>73</v>
-      </c>
-      <c r="O5" s="298" t="s">
-        <v>66</v>
-      </c>
-      <c r="P5" s="299" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q5" s="297" t="s">
-        <v>60</v>
-      </c>
-      <c r="R5" s="298" t="s">
-        <v>61</v>
-      </c>
-      <c r="S5" s="299" t="s">
-        <v>58</v>
+      <c r="S5" s="278" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.3">
@@ -4211,22 +4191,22 @@
         <v>0.1</v>
       </c>
       <c r="N6" s="233"/>
-      <c r="O6" s="234">
+      <c r="O6" s="231">
         <v>4.7E-2</v>
       </c>
-      <c r="P6" s="235"/>
+      <c r="P6" s="234"/>
       <c r="Q6" s="229">
         <v>4.7E-2</v>
       </c>
-      <c r="R6" s="236">
+      <c r="R6" s="235">
         <v>4.7E-2</v>
       </c>
-      <c r="S6" s="237">
+      <c r="S6" s="236">
         <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="238" t="s">
+      <c r="B7" s="237" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -4252,7 +4232,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="147">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N7" s="178"/>
       <c r="O7" s="54"/>
@@ -4264,7 +4244,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="239" t="s">
+      <c r="B8" s="238" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -4305,7 +4285,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="240" t="s">
+      <c r="B9" s="239" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4333,7 +4313,7 @@
       <c r="S9" s="204"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="241" t="s">
+      <c r="B10" s="240" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -4361,7 +4341,7 @@
       <c r="S10" s="205"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="238" t="s">
+      <c r="B11" s="237" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -4388,7 +4368,6 @@
         <v>2.1</v>
       </c>
       <c r="N11" s="185">
-        <f>1.7*2</f>
         <v>3.4</v>
       </c>
       <c r="O11" s="54"/>
@@ -4398,7 +4377,7 @@
       <c r="S11" s="206"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="239" t="s">
+      <c r="B12" s="238" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -4428,7 +4407,7 @@
       <c r="S12" s="207"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="242" t="s">
+      <c r="B13" s="241" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="77" t="s">
@@ -4456,7 +4435,7 @@
       <c r="S13" s="208"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B14" s="243" t="s">
+      <c r="B14" s="242" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="78" t="s">
@@ -4485,8 +4464,8 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B15" s="242" t="s">
-        <v>78</v>
+      <c r="B15" s="241" t="s">
+        <v>76</v>
       </c>
       <c r="C15" s="77" t="s">
         <v>2</v>
@@ -4506,7 +4485,7 @@
       <c r="L15" s="40"/>
       <c r="M15" s="161"/>
       <c r="N15" s="186">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O15" s="41">
         <v>20</v>
@@ -4521,7 +4500,7 @@
       <c r="S15" s="211"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B16" s="238" t="s">
+      <c r="B16" s="237" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -4531,37 +4510,35 @@
         <v>17</v>
       </c>
       <c r="E16" s="125" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>34</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" s="126"/>
       <c r="J16" s="162"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="163"/>
-      <c r="N16" s="188" t="s">
-        <v>35</v>
-      </c>
+      <c r="N16" s="188"/>
       <c r="O16" s="15"/>
       <c r="P16" s="126"/>
       <c r="Q16" s="212" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R16" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S16" s="213"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B17" s="244" t="s">
+      <c r="B17" s="243" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -4571,37 +4548,35 @@
         <v>17</v>
       </c>
       <c r="E17" s="127" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I17" s="128"/>
       <c r="J17" s="164"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="165"/>
-      <c r="N17" s="189" t="s">
-        <v>46</v>
-      </c>
+      <c r="N17" s="189"/>
       <c r="O17" s="16"/>
       <c r="P17" s="128"/>
       <c r="Q17" s="214" t="s">
+        <v>41</v>
+      </c>
+      <c r="R17" s="26" t="s">
         <v>42</v>
-      </c>
-      <c r="R17" s="26" t="s">
-        <v>43</v>
       </c>
       <c r="S17" s="215"/>
     </row>
     <row r="18" spans="2:19" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="245" t="s">
+      <c r="B18" s="244" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="79" t="s">
@@ -4627,9 +4602,7 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="167"/>
-      <c r="N18" s="190">
-        <v>0</v>
-      </c>
+      <c r="N18" s="190"/>
       <c r="O18" s="17"/>
       <c r="P18" s="130"/>
       <c r="Q18" s="216">
@@ -4641,7 +4614,7 @@
       <c r="S18" s="217"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B19" s="242" t="s">
+      <c r="B19" s="241" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="77" t="s">
@@ -4669,8 +4642,8 @@
       <c r="S19" s="218"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="246" t="s">
-        <v>41</v>
+      <c r="B20" s="245" t="s">
+        <v>40</v>
       </c>
       <c r="C20" s="90" t="s">
         <v>2</v>
@@ -4697,7 +4670,7 @@
       <c r="S20" s="219"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="240" t="s">
+      <c r="B21" s="239" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -4729,7 +4702,7 @@
       <c r="S21" s="220"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="247" t="s">
+      <c r="B22" s="246" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="84" t="s">
@@ -4739,8 +4712,8 @@
         <v>10</v>
       </c>
       <c r="E22" s="138">
-        <f>0.1*6</f>
-        <v>0.60000000000000009</v>
+        <f>0.1*3</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="F22" s="89"/>
       <c r="G22" s="85"/>
@@ -4748,12 +4721,12 @@
         <v>1</v>
       </c>
       <c r="I22" s="140">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J22" s="174"/>
       <c r="K22" s="139">
-        <f>0.8*1.4*6</f>
-        <v>6.7199999999999989</v>
+        <f>0.8*1.4*3</f>
+        <v>3.3599999999999994</v>
       </c>
       <c r="L22" s="87"/>
       <c r="M22" s="175"/>
@@ -4763,65 +4736,65 @@
       <c r="Q22" s="174"/>
       <c r="R22" s="86"/>
       <c r="S22" s="140">
-        <f>0.8*1.4*6</f>
-        <v>6.7199999999999989</v>
+        <f>0.8*1.4*3</f>
+        <v>3.3599999999999994</v>
       </c>
     </row>
     <row r="23" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="248" t="s">
+      <c r="B23" s="247" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="249" t="s">
+      <c r="C23" s="248" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="250" t="s">
+      <c r="D23" s="249" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="141">
-        <f>0.1*6</f>
-        <v>0.60000000000000009</v>
+        <f>0.1*3</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="F23" s="142"/>
       <c r="G23" s="143">
-        <f>0.1*6</f>
-        <v>0.60000000000000009</v>
+        <f>0.1*3</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="H23" s="144"/>
       <c r="I23" s="145"/>
       <c r="J23" s="176"/>
       <c r="K23" s="143">
-        <f>0.1*0.8*7*6</f>
-        <v>3.3600000000000003</v>
+        <f>0.1*0.8*7*3</f>
+        <v>1.6800000000000002</v>
       </c>
       <c r="L23" s="143">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M23" s="177">
-        <f>0.1*0.8*7*6</f>
-        <v>3.3600000000000003</v>
+        <f>0.1*0.8*7*3</f>
+        <v>1.6800000000000002</v>
       </c>
       <c r="N23" s="199"/>
       <c r="O23" s="143">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P23" s="200"/>
       <c r="Q23" s="176"/>
       <c r="R23" s="143">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S23" s="177">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:19" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B25" s="278" t="s">
+      <c r="B25" s="280" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="279"/>
-      <c r="D25" s="279"/>
-      <c r="E25" s="279"/>
-      <c r="F25" s="280"/>
+      <c r="C25" s="281"/>
+      <c r="D25" s="281"/>
+      <c r="E25" s="281"/>
+      <c r="F25" s="282"/>
     </row>
     <row r="26" spans="2:19" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
@@ -4830,22 +4803,22 @@
       </c>
       <c r="C27" s="98"/>
       <c r="D27" s="98"/>
-      <c r="E27" s="281" t="s">
+      <c r="E27" s="283" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="282"/>
+      <c r="F27" s="284"/>
     </row>
     <row r="28" spans="2:19" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B29" s="97" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="96"/>
       <c r="D29" s="96"/>
-      <c r="E29" s="277" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="277"/>
+      <c r="E29" s="279" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="279"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4891,17 +4864,17 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update threshold values workbook
</commit_message>
<xml_diff>
--- a/LifespanDesign/.templates/threshold_values.xlsx
+++ b/LifespanDesign/.templates/threshold_values.xlsx
@@ -311,9 +311,6 @@
     <t>TERRAFORMING</t>
   </si>
   <si>
-    <t>MAINTENANCE</t>
-  </si>
-  <si>
     <t>BIOENGINEERING (OTHER)</t>
   </si>
   <si>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>Incorporation of fine sediment</t>
+  </si>
+  <si>
+    <t>CONNECTIVITY</t>
   </si>
 </sst>
 </file>
@@ -3968,7 +3968,7 @@
   <dimension ref="B1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="Q3" sqref="Q3:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4009,12 +4009,12 @@
       <c r="L2" s="291"/>
       <c r="M2" s="292"/>
       <c r="N2" s="293" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O2" s="294"/>
       <c r="P2" s="295"/>
       <c r="Q2" s="296" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="R2" s="297"/>
       <c r="S2" s="298"/>
@@ -4044,7 +4044,7 @@
       </c>
       <c r="R3" s="286"/>
       <c r="S3" s="275" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="25.5" x14ac:dyDescent="0.3">
@@ -4067,10 +4067,10 @@
         <v>47</v>
       </c>
       <c r="H4" s="271" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="272" t="s">
         <v>78</v>
-      </c>
-      <c r="I4" s="272" t="s">
-        <v>79</v>
       </c>
       <c r="J4" s="269" t="s">
         <v>50</v>
@@ -4088,10 +4088,10 @@
         <v>72</v>
       </c>
       <c r="O4" s="271" t="s">
+        <v>79</v>
+      </c>
+      <c r="P4" s="272" t="s">
         <v>80</v>
-      </c>
-      <c r="P4" s="272" t="s">
-        <v>81</v>
       </c>
       <c r="Q4" s="274" t="s">
         <v>48</v>
@@ -4100,7 +4100,7 @@
         <v>49</v>
       </c>
       <c r="S4" s="272" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -4465,7 +4465,7 @@
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B15" s="241" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="77" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Edit theshold value: Streamwood
</commit_message>
<xml_diff>
--- a/LifespanDesign/.templates/threshold_values.xlsx
+++ b/LifespanDesign/.templates/threshold_values.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\RiverArchitect\LifespanDesign\.templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\RA_program\LifespanDesign\.templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3954,7 +3954,7 @@
   <dimension ref="B1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4354,7 +4354,7 @@
         <v>2.1</v>
       </c>
       <c r="N11" s="176">
-        <v>3.4</v>
+        <v>3.34</v>
       </c>
       <c r="O11" s="179"/>
       <c r="P11" s="180"/>

</xml_diff>

<commit_message>
Changed terminology: Bioengineering to nature-based eng.
</commit_message>
<xml_diff>
--- a/LifespanDesign/.templates/threshold_values.xlsx
+++ b/LifespanDesign/.templates/threshold_values.xlsx
@@ -305,9 +305,6 @@
     <t>TERRAFORMING</t>
   </si>
   <si>
-    <t>BIOENGINEERING (OTHER)</t>
-  </si>
-  <si>
     <t>Design map frequency threshold</t>
   </si>
   <si>
@@ -338,7 +335,10 @@
     <t>Bool</t>
   </si>
   <si>
-    <t>Other bioeng.</t>
+    <t>Other nature-based eng.</t>
+  </si>
+  <si>
+    <t>NATURE-BASED (OTHER)</t>
   </si>
 </sst>
 </file>
@@ -3954,7 +3954,7 @@
   <dimension ref="B1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3995,12 +3995,12 @@
       <c r="L2" s="284"/>
       <c r="M2" s="285"/>
       <c r="N2" s="286" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="O2" s="287"/>
       <c r="P2" s="288"/>
       <c r="Q2" s="289" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R2" s="290"/>
       <c r="S2" s="291"/>
@@ -4030,7 +4030,7 @@
       </c>
       <c r="R3" s="279"/>
       <c r="S3" s="95" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:19" ht="25.5" x14ac:dyDescent="0.3">
@@ -4053,10 +4053,10 @@
         <v>45</v>
       </c>
       <c r="H4" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="94" t="s">
         <v>75</v>
-      </c>
-      <c r="I4" s="94" t="s">
-        <v>76</v>
       </c>
       <c r="J4" s="243" t="s">
         <v>48</v>
@@ -4074,10 +4074,10 @@
         <v>70</v>
       </c>
       <c r="O4" s="93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P4" s="94" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q4" s="236" t="s">
         <v>46</v>
@@ -4086,7 +4086,7 @@
         <v>47</v>
       </c>
       <c r="S4" s="94" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -4451,7 +4451,7 @@
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B15" s="68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>2</v>
@@ -4763,7 +4763,7 @@
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B24" s="249" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="250" t="s">
         <v>16</v>
@@ -4819,7 +4819,7 @@
     </row>
     <row r="25" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="252" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="253" t="s">
         <v>16</v>
@@ -4952,7 +4952,7 @@
         <v>35</v>
       </c>
       <c r="D3" s="255" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
'Depth to groundwater' changed to 'depth to water table' in code and spreadsheet.
</commit_message>
<xml_diff>
--- a/LifespanDesign/.templates/threshold_values.xlsx
+++ b/LifespanDesign/.templates/threshold_values.xlsx
@@ -1,36 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\RA_program\LifespanDesign\.templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\PycharmProjects\pythonProject\LifespanDesign\.templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0808BCA0-F03C-44E6-A926-00971FFDD115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="14280"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="thresholds" sheetId="1" r:id="rId1"/>
     <sheet name=".templates" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sebastian Schwindt</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -103,12 +113,6 @@
     <t>Critical dimensionless bed shear stress</t>
   </si>
   <si>
-    <t>Depth to groundwater (min)</t>
-  </si>
-  <si>
-    <t>Depth to groundwater (max)</t>
-  </si>
-  <si>
     <t>Froude number</t>
   </si>
   <si>
@@ -339,12 +343,18 @@
   </si>
   <si>
     <t>NATURE-BASED (OTHER)</t>
+  </si>
+  <si>
+    <t>Depth to water table (min)</t>
+  </si>
+  <si>
+    <t>Depth to water table (max)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -2794,7 +2804,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="292">
+  <cellXfs count="294">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3625,6 +3635,8 @@
     <xf numFmtId="0" fontId="14" fillId="10" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27" customBuiltin="1"/>
@@ -3669,20 +3681,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:B5" totalsRowShown="0">
-  <autoFilter ref="B3:B5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:B5" totalsRowShown="0">
+  <autoFilter ref="B3:B5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="units"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="units"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D3:D5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="D3:D5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="D3:D5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="D3:D5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Bool" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bool" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3950,57 +3962,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="5.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.875" style="2" customWidth="1"/>
-    <col min="8" max="9" width="9.25" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.75" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="7.125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.5" style="2" customWidth="1"/>
-    <col min="17" max="18" width="9.125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="13.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="9.21875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" style="2" customWidth="1"/>
+    <col min="17" max="18" width="9.109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="13.88671875" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:19" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:19" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="280" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F2" s="281"/>
       <c r="G2" s="281"/>
       <c r="H2" s="281"/>
       <c r="I2" s="282"/>
       <c r="J2" s="283" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K2" s="284"/>
       <c r="L2" s="284"/>
       <c r="M2" s="285"/>
       <c r="N2" s="286" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O2" s="287"/>
       <c r="P2" s="288"/>
       <c r="Q2" s="289" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="R2" s="290"/>
       <c r="S2" s="291"/>
@@ -4008,10 +4020,10 @@
     <row r="3" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="77"/>
       <c r="C3" s="78" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="79" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="80"/>
       <c r="F3" s="81"/>
@@ -4026,126 +4038,126 @@
       <c r="O3" s="82"/>
       <c r="P3" s="84"/>
       <c r="Q3" s="278" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R3" s="279"/>
       <c r="S3" s="95" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B4" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="92" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="92" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="94" t="s">
         <v>73</v>
       </c>
+      <c r="J4" s="243" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="244" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="244" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="245" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q4" s="236" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" s="237" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" s="94" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="4" spans="2:19" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="88" t="s">
+    <row r="5" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="85" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="86" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="87" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="97" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="97" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="97" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="98" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="246" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="247" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="247" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="248" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="89" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="91" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="92" t="s">
+      <c r="O5" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="P5" s="98" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q5" s="238" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" s="239" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="93" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="94" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" s="243" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="244" t="s">
-        <v>49</v>
-      </c>
-      <c r="L4" s="244" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="245" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="91" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" s="93" t="s">
-        <v>76</v>
-      </c>
-      <c r="P4" s="94" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q4" s="236" t="s">
-        <v>46</v>
-      </c>
-      <c r="R4" s="237" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4" s="94" t="s">
-        <v>77</v>
-      </c>
     </row>
-    <row r="5" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="85" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="86" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="87" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="96" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="97" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="97" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="97" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="98" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="246" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="247" t="s">
-        <v>59</v>
-      </c>
-      <c r="L5" s="247" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="248" t="s">
-        <v>61</v>
-      </c>
-      <c r="N5" s="96" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="97" t="s">
-        <v>62</v>
-      </c>
-      <c r="P5" s="98" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q5" s="238" t="s">
-        <v>56</v>
-      </c>
-      <c r="R5" s="239" t="s">
-        <v>57</v>
-      </c>
-      <c r="S5" s="98" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="61" t="s">
         <v>4</v>
       </c>
@@ -4153,7 +4165,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="63" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6" s="231">
         <v>4.7E-2</v>
@@ -4191,15 +4203,15 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="64" t="s">
-        <v>5</v>
+    <row r="7" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B7" s="292" t="s">
+        <v>82</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" s="219"/>
       <c r="F7" s="177"/>
@@ -4229,15 +4241,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="65" t="s">
-        <v>6</v>
+    <row r="8" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B8" s="293" t="s">
+        <v>83</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" s="223"/>
       <c r="F8" s="187"/>
@@ -4270,15 +4282,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B9" s="66" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="195"/>
       <c r="F9" s="196">
@@ -4298,15 +4310,15 @@
       <c r="R9" s="204"/>
       <c r="S9" s="205"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B10" s="67" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" s="206"/>
       <c r="F10" s="207">
@@ -4326,7 +4338,7 @@
       <c r="R10" s="215"/>
       <c r="S10" s="216"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B11" s="64" t="s">
         <v>0</v>
       </c>
@@ -4334,7 +4346,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E11" s="176"/>
       <c r="F11" s="177"/>
@@ -4362,7 +4374,7 @@
       <c r="R11" s="184"/>
       <c r="S11" s="185"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12" s="65" t="s">
         <v>3</v>
       </c>
@@ -4370,7 +4382,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E12" s="186">
         <v>0.1</v>
@@ -4392,15 +4404,15 @@
       <c r="R12" s="106"/>
       <c r="S12" s="194"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B13" s="68" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E13" s="41"/>
       <c r="F13" s="13"/>
@@ -4420,15 +4432,15 @@
       <c r="R13" s="15"/>
       <c r="S13" s="58"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="69" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" s="164"/>
       <c r="F14" s="165"/>
@@ -4449,15 +4461,15 @@
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B15" s="68" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" s="105">
         <v>5</v>
@@ -4485,27 +4497,27 @@
       </c>
       <c r="S15" s="59"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B16" s="64" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E16" s="143" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F16" s="144" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16" s="145" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H16" s="146" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I16" s="147"/>
       <c r="J16" s="148"/>
@@ -4516,34 +4528,34 @@
       <c r="O16" s="150"/>
       <c r="P16" s="147"/>
       <c r="Q16" s="99" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R16" s="100" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S16" s="151"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B17" s="70" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F17" s="153" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G17" s="154" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H17" s="155" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I17" s="156"/>
       <c r="J17" s="157"/>
@@ -4554,22 +4566,22 @@
       <c r="O17" s="159"/>
       <c r="P17" s="156"/>
       <c r="Q17" s="160" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R17" s="161" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="S17" s="162"/>
     </row>
-    <row r="18" spans="2:19" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:19" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B18" s="71" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E18" s="130">
         <v>1</v>
@@ -4599,15 +4611,15 @@
       </c>
       <c r="S18" s="138"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B19" s="68" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19" s="41"/>
       <c r="F19" s="13"/>
@@ -4627,15 +4639,15 @@
       <c r="R19" s="15"/>
       <c r="S19" s="58"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B20" s="72" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E20" s="44"/>
       <c r="F20" s="27"/>
@@ -4655,15 +4667,15 @@
       <c r="R20" s="24"/>
       <c r="S20" s="60"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B21" s="66" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="39" t="s">
         <v>16</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>18</v>
       </c>
       <c r="E21" s="117"/>
       <c r="F21" s="118"/>
@@ -4687,15 +4699,15 @@
       <c r="R21" s="125"/>
       <c r="S21" s="119"/>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B22" s="73" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E22" s="54">
         <f>0.1*3</f>
@@ -4723,15 +4735,15 @@
         <v>3.3599999999999994</v>
       </c>
     </row>
-    <row r="23" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="74" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" s="75" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="76" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E23" s="56">
         <f>0.1*3</f>
@@ -4761,15 +4773,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B24" s="249" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="250" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="251" t="s">
         <v>16</v>
-      </c>
-      <c r="D24" s="251" t="s">
-        <v>18</v>
       </c>
       <c r="E24" s="256" t="b">
         <v>1</v>
@@ -4817,15 +4829,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="252" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" s="253" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="254" t="s">
         <v>16</v>
-      </c>
-      <c r="D25" s="254" t="s">
-        <v>18</v>
       </c>
       <c r="E25" s="266" t="b">
         <v>1</v>
@@ -4873,25 +4885,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:19" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:19" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27" s="277" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C27" s="277"/>
       <c r="D27" s="277"/>
       <c r="E27" s="277"/>
       <c r="F27" s="277"/>
     </row>
-    <row r="28" spans="2:19" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:19" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
       <c r="E29" s="276" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F29" s="276"/>
     </row>
@@ -4916,13 +4928,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'.templates'!$B$4:$B$5</xm:f>
           </x14:formula1>
           <xm:sqref>E29:F29</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'.templates'!$D$4:$D$5</xm:f>
           </x14:formula1>
@@ -4935,37 +4947,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="255" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="255" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" s="255" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Reading threshold_values dynamically. Few changes in threshold excel file.
</commit_message>
<xml_diff>
--- a/LifespanDesign/.templates/threshold_values.xlsx
+++ b/LifespanDesign/.templates/threshold_values.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b8ba4e84fea5adb/Desktop/program-master (3)/program-master/LifespanDesign/.templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\PycharmProjects\pythonProject\LifespanDesign\.templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="13_ncr:1_{0808BCA0-F03C-44E6-A926-00971FFDD115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DFD0391-D354-41D2-A264-71590E2A9D18}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC3044F-AEAF-4A9B-9C73-9676853098CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,9 +183,6 @@
 (0 = avoidance, 1 = relevance)</t>
   </si>
   <si>
-    <t>DO NOT DELETE, SHIFT, COPY OR INSERT CELLS, ROWS AND COLUMNS</t>
-  </si>
-  <si>
     <t>bedrock, hillside</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>bed shear stress</t>
+  </si>
+  <si>
+    <t>YOU CAN ADD FURTHER THRESHOLD ATTRIBUTES AND FEATURES</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3946,6 +3946,61 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="175" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="176" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="176" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="177" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="172" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="178" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="179" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="180" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="181" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="182" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="183" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="157" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="163" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="184" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="175" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3994,62 +4049,7 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="153" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="175" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="176" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="176" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="177" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="172" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="178" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="179" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="180" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="181" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="182" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="183" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="157" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="163" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="184" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="175" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27" customBuiltin="1"/>
@@ -4059,6 +4059,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -4070,15 +4079,6 @@
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4104,10 +4104,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="D3:D5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="D3:D5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="D3:D5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bool" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bool" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4378,8 +4378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4411,37 +4411,37 @@
   <sheetData>
     <row r="1" spans="2:25" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:25" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="299" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="300"/>
-      <c r="G2" s="300"/>
-      <c r="H2" s="300"/>
-      <c r="I2" s="301"/>
-      <c r="J2" s="308" t="s">
-        <v>83</v>
-      </c>
-      <c r="K2" s="309"/>
-      <c r="L2" s="309"/>
-      <c r="M2" s="309"/>
-      <c r="N2" s="310"/>
-      <c r="O2" s="308" t="s">
-        <v>85</v>
-      </c>
-      <c r="P2" s="309"/>
-      <c r="Q2" s="309"/>
-      <c r="R2" s="309"/>
-      <c r="S2" s="310"/>
-      <c r="T2" s="302" t="s">
-        <v>80</v>
-      </c>
-      <c r="U2" s="303"/>
-      <c r="V2" s="304"/>
-      <c r="W2" s="305" t="s">
-        <v>75</v>
-      </c>
-      <c r="X2" s="306"/>
-      <c r="Y2" s="307"/>
+      <c r="E2" s="318" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="319"/>
+      <c r="G2" s="319"/>
+      <c r="H2" s="319"/>
+      <c r="I2" s="320"/>
+      <c r="J2" s="327" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" s="328"/>
+      <c r="L2" s="328"/>
+      <c r="M2" s="328"/>
+      <c r="N2" s="329"/>
+      <c r="O2" s="327" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="328"/>
+      <c r="Q2" s="328"/>
+      <c r="R2" s="328"/>
+      <c r="S2" s="329"/>
+      <c r="T2" s="321" t="s">
+        <v>79</v>
+      </c>
+      <c r="U2" s="322"/>
+      <c r="V2" s="323"/>
+      <c r="W2" s="324" t="s">
+        <v>74</v>
+      </c>
+      <c r="X2" s="325"/>
+      <c r="Y2" s="326"/>
     </row>
     <row r="3" spans="2:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="71"/>
@@ -4469,17 +4469,17 @@
       <c r="T3" s="74"/>
       <c r="U3" s="76"/>
       <c r="V3" s="78"/>
-      <c r="W3" s="297" t="s">
+      <c r="W3" s="316" t="s">
         <v>22</v>
       </c>
-      <c r="X3" s="298"/>
+      <c r="X3" s="317"/>
       <c r="Y3" s="89" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="2:25" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B4" s="82" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="83" t="s">
         <v>6</v>
@@ -4488,72 +4488,72 @@
         <v>15</v>
       </c>
       <c r="E4" s="85" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="86" t="s">
+      <c r="H4" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="88" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="232" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" s="203" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="203" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="203" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="204" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="248" t="s">
+        <v>85</v>
+      </c>
+      <c r="P4" s="293" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q4" s="232" t="s">
+        <v>88</v>
+      </c>
+      <c r="R4" s="292" t="s">
+        <v>90</v>
+      </c>
+      <c r="S4" s="204" t="s">
+        <v>93</v>
+      </c>
+      <c r="T4" s="85" t="s">
+        <v>66</v>
+      </c>
+      <c r="U4" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="V4" s="88" t="s">
+        <v>78</v>
+      </c>
+      <c r="W4" s="197" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="87" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="88" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="232" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" s="203" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="203" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="203" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="204" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="248" t="s">
-        <v>86</v>
-      </c>
-      <c r="P4" s="293" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q4" s="232" t="s">
-        <v>89</v>
-      </c>
-      <c r="R4" s="292" t="s">
-        <v>91</v>
-      </c>
-      <c r="S4" s="204" t="s">
-        <v>94</v>
-      </c>
-      <c r="T4" s="85" t="s">
-        <v>67</v>
-      </c>
-      <c r="U4" s="87" t="s">
+      <c r="X4" s="198" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y4" s="88" t="s">
         <v>73</v>
-      </c>
-      <c r="V4" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="W4" s="197" t="s">
-        <v>43</v>
-      </c>
-      <c r="X4" s="198" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y4" s="88" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="80" t="s">
         <v>6</v>
@@ -4562,103 +4562,103 @@
         <v>15</v>
       </c>
       <c r="E5" s="90" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="199" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="290" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="278" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="278" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="205" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" s="288" t="s">
+        <v>85</v>
+      </c>
+      <c r="P5" s="291" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q5" s="291" t="s">
+        <v>89</v>
+      </c>
+      <c r="R5" s="291" t="s">
+        <v>91</v>
+      </c>
+      <c r="S5" s="205" t="s">
+        <v>92</v>
+      </c>
+      <c r="T5" s="90" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" s="199" t="s">
+        <v>52</v>
+      </c>
+      <c r="X5" s="200" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y5" s="92" t="s">
         <v>50</v>
-      </c>
-      <c r="F5" s="91" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="91" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="91" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="92" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" s="199" t="s">
-        <v>84</v>
-      </c>
-      <c r="K5" s="290" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="278" t="s">
-        <v>56</v>
-      </c>
-      <c r="M5" s="278" t="s">
-        <v>57</v>
-      </c>
-      <c r="N5" s="205" t="s">
-        <v>58</v>
-      </c>
-      <c r="O5" s="288" t="s">
-        <v>86</v>
-      </c>
-      <c r="P5" s="291" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q5" s="291" t="s">
-        <v>90</v>
-      </c>
-      <c r="R5" s="291" t="s">
-        <v>92</v>
-      </c>
-      <c r="S5" s="205" t="s">
-        <v>93</v>
-      </c>
-      <c r="T5" s="90" t="s">
-        <v>66</v>
-      </c>
-      <c r="U5" s="91" t="s">
-        <v>59</v>
-      </c>
-      <c r="V5" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="W5" s="199" t="s">
-        <v>53</v>
-      </c>
-      <c r="X5" s="200" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y5" s="92" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="329" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="330" t="s">
+      <c r="B6" s="312" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="313" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="311"/>
-      <c r="F6" s="322"/>
-      <c r="G6" s="322"/>
-      <c r="H6" s="321"/>
-      <c r="I6" s="313"/>
-      <c r="J6" s="312"/>
-      <c r="K6" s="325"/>
-      <c r="L6" s="314"/>
-      <c r="M6" s="326"/>
-      <c r="N6" s="315"/>
-      <c r="O6" s="314"/>
-      <c r="P6" s="324"/>
-      <c r="Q6" s="327"/>
-      <c r="R6" s="314"/>
-      <c r="S6" s="328"/>
-      <c r="T6" s="311"/>
-      <c r="U6" s="319"/>
-      <c r="V6" s="320"/>
-      <c r="W6" s="316"/>
-      <c r="X6" s="317"/>
-      <c r="Y6" s="320"/>
+      <c r="E6" s="295"/>
+      <c r="F6" s="306"/>
+      <c r="G6" s="306"/>
+      <c r="H6" s="305"/>
+      <c r="I6" s="297"/>
+      <c r="J6" s="296"/>
+      <c r="K6" s="308"/>
+      <c r="L6" s="298"/>
+      <c r="M6" s="309"/>
+      <c r="N6" s="299"/>
+      <c r="O6" s="298"/>
+      <c r="P6" s="307"/>
+      <c r="Q6" s="310"/>
+      <c r="R6" s="298"/>
+      <c r="S6" s="311"/>
+      <c r="T6" s="295"/>
+      <c r="U6" s="303"/>
+      <c r="V6" s="304"/>
+      <c r="W6" s="300"/>
+      <c r="X6" s="301"/>
+      <c r="Y6" s="304"/>
     </row>
     <row r="7" spans="2:25" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B7" s="318" t="s">
+      <c r="B7" s="302" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="57" t="s">
@@ -4717,7 +4717,7 @@
     </row>
     <row r="8" spans="2:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" s="229" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>2</v>
@@ -4769,7 +4769,7 @@
     </row>
     <row r="9" spans="2:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B9" s="230" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>2</v>
@@ -4857,7 +4857,7 @@
       <c r="Y10" s="170"/>
     </row>
     <row r="11" spans="2:25" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="323" t="s">
+      <c r="B11" s="330" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -5049,7 +5049,7 @@
     </row>
     <row r="16" spans="2:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B16" s="294" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>2</v>
@@ -5100,16 +5100,16 @@
         <v>15</v>
       </c>
       <c r="E17" s="119" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="120" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="121" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="122" t="s">
         <v>29</v>
-      </c>
-      <c r="H17" s="122" t="s">
-        <v>30</v>
       </c>
       <c r="I17" s="123"/>
       <c r="J17" s="241"/>
@@ -5126,10 +5126,10 @@
       <c r="U17" s="125"/>
       <c r="V17" s="123"/>
       <c r="W17" s="93" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X17" s="94" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y17" s="126"/>
     </row>
@@ -5144,16 +5144,16 @@
         <v>15</v>
       </c>
       <c r="E18" s="127" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="128" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="129" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" s="130" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I18" s="131"/>
       <c r="J18" s="242"/>
@@ -5170,10 +5170,10 @@
       <c r="U18" s="133"/>
       <c r="V18" s="131"/>
       <c r="W18" s="134" t="s">
+        <v>35</v>
+      </c>
+      <c r="X18" s="135" t="s">
         <v>36</v>
-      </c>
-      <c r="X18" s="135" t="s">
-        <v>37</v>
       </c>
       <c r="Y18" s="136"/>
     </row>
@@ -5257,7 +5257,7 @@
     </row>
     <row r="21" spans="2:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B21" s="66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>2</v>
@@ -5415,7 +5415,7 @@
     </row>
     <row r="25" spans="2:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B25" s="206" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="207" t="s">
         <v>14</v>
@@ -5485,7 +5485,7 @@
     </row>
     <row r="26" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="209" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="210" t="s">
         <v>14</v>
@@ -5555,25 +5555,25 @@
     </row>
     <row r="27" spans="2:25" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B28" s="296" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="296"/>
-      <c r="D28" s="296"/>
-      <c r="E28" s="296"/>
-      <c r="F28" s="296"/>
+      <c r="B28" s="315" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="315"/>
+      <c r="D28" s="315"/>
+      <c r="E28" s="315"/>
+      <c r="F28" s="315"/>
     </row>
     <row r="29" spans="2:25" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" s="27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="295" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="295"/>
+      <c r="E30" s="314" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="314"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5587,7 +5587,7 @@
     <mergeCell ref="O2:S2"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:Y26">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>NOT(ISBLANK(E7))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5630,15 +5630,15 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="212" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="212" t="b">
         <v>0</v>
@@ -5646,7 +5646,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="212" t="b">
         <v>1</v>

</xml_diff>